<commit_message>
Update TR2 RA judge workflow.
</commit_message>
<xml_diff>
--- a/td_toolkits_v3/static/sheets/reliability_upload_template.xlsx
+++ b/td_toolkits_v3/static/sheets/reliability_upload_template.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dimsp\Documents\Projects\td_toolkits_v3\td_toolkits_v3\static\sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FC1261-02C7-4885-B4F5-C3D44E5A847C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="37690" windowHeight="21820" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Adhesion" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="LTO" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="LTS" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="PCT" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Seal WVTR" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Δangle" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="U-Shape AC" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="VHR" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Adhesion" sheetId="1" r:id="rId1"/>
+    <sheet name="LTO" sheetId="2" r:id="rId2"/>
+    <sheet name="LTS" sheetId="3" r:id="rId3"/>
+    <sheet name="PCT" sheetId="4" r:id="rId4"/>
+    <sheet name="Seal WVTR" sheetId="5" r:id="rId5"/>
+    <sheet name="Δangle" sheetId="6" r:id="rId6"/>
+    <sheet name="U-Shape AC" sheetId="7" r:id="rId7"/>
+    <sheet name="VHR" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Adhesion!$A$1:$K$34</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">PCT!$A$1:$I$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Seal WVTR'!$A$1:$L$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">VHR!$A$1:$K$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Adhesion!$A$1:$K$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">PCT!$A$1:$I$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Seal WVTR'!$A$1:$L$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7">VHR!$A$1:$K$32</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,24 +37,24 @@
 </workbook>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
-            <b val="true"/>
+            <b/>
             <sz val="9"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">NA: fresh LC
+          <t>NA: fresh LC
 Seal name: jar test</t>
         </r>
       </text>
@@ -59,44 +64,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="35">
   <si>
-    <t xml:space="preserve">項目</t>
+    <t>項目</t>
   </si>
   <si>
-    <t xml:space="preserve">LC</t>
+    <t>LC</t>
   </si>
   <si>
-    <t xml:space="preserve">PI</t>
+    <t>PI</t>
   </si>
   <si>
-    <t xml:space="preserve">Seal</t>
+    <t>Seal</t>
   </si>
   <si>
-    <t xml:space="preserve">Y軸數值</t>
+    <t>Y軸數值</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit</t>
+    <t>Unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition:
+    <t>Measure condition:
 Adhesion介面(T/C)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition:
+    <t>Measure condition:
 測試手法</t>
   </si>
   <si>
-    <t xml:space="preserve">Remark:Peeling介面(T/C)</t>
+    <t>Remark:Peeling介面(T/C)</t>
   </si>
   <si>
-    <t xml:space="preserve">Vender</t>
+    <t>Vender</t>
   </si>
   <si>
-    <t xml:space="preserve">File source</t>
+    <t>File source</t>
   </si>
   <si>
-    <t xml:space="preserve">Sealant</t>
+    <t>Sealant</t>
   </si>
   <si>
     <r>
@@ -107,7 +112,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">LTO result
+      <t>LTO result
 (</t>
     </r>
     <r>
@@ -118,7 +123,7 @@
         <family val="3"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">有黑屏</t>
+      <t>有黑屏</t>
     </r>
     <r>
       <rPr>
@@ -128,19 +133,19 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">: NG)</t>
+      <t>: NG)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (Bulk/Test Cell)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (SLV%, Fresh=100%)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (Jar test add on Sealant)</t>
   </si>
   <si>
@@ -152,7 +157,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Measure condition
+      <t>Measure condition
 (</t>
     </r>
     <r>
@@ -163,7 +168,7 @@
         <family val="1"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">℃</t>
+      <t>℃</t>
     </r>
     <r>
       <rPr>
@@ -173,145 +178,129 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)</t>
+      <t>)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">LTS result
+    <t>LTS result
 (1st NG Day)</t>
   </si>
   <si>
-    <t xml:space="preserve">Y軸數值 
+    <t>Y軸數值 
 (Bubble 5% hours)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 測試條件</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition:
+    <t>Measure condition:
 test vehicle</t>
   </si>
   <si>
-    <t xml:space="preserve">Y軸項目</t>
+    <t>Y軸項目</t>
   </si>
   <si>
-    <t xml:space="preserve">Time</t>
+    <t>Time</t>
   </si>
   <si>
-    <t xml:space="preserve">溫度(°C)</t>
+    <t>溫度(°C)</t>
   </si>
   <si>
-    <t xml:space="preserve">濕度(%)</t>
+    <t>濕度(%)</t>
   </si>
   <si>
-    <t xml:space="preserve">膜厚(um)</t>
+    <t>膜厚(um)</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Y</t>
+      <t>Y</t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="細明體"/>
         <family val="3"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">軸數值</t>
+      <t>軸數值</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (Voltage:V)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (Frequence:hz)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (Time:hr)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (溫度:oC)</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Y</t>
+      <t>Y</t>
     </r>
     <r>
       <rPr>
-        <b val="true"/>
+        <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="細明體"/>
         <family val="3"/>
         <charset val="136"/>
       </rPr>
-      <t xml:space="preserve">軸數值
+      <t>軸數值
 (取中位數)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">VHR
+    <t>VHR
 (Heat)</t>
   </si>
   <si>
-    <t xml:space="preserve">Measure condition
+    <t>Measure condition
 (UV aging)</t>
+  </si>
+  <si>
+    <t>Batch</t>
+    <phoneticPr fontId="22" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -355,18 +344,6 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF3333FF"/>
       <name val="新細明體"/>
@@ -408,7 +385,7 @@
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
@@ -416,7 +393,7 @@
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -424,7 +401,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="細明體"/>
@@ -432,7 +409,7 @@
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="新細明體"/>
@@ -440,21 +417,21 @@
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
@@ -462,12 +439,25 @@
       <charset val="136"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="5">
@@ -497,367 +487,287 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="72">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="一般 2" xfId="20"/>
-    <cellStyle name="百分比 2" xfId="21"/>
+  <cellStyles count="3">
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="百分比 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -916,14 +826,30 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF3333FF"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>303840</xdr:colOff>
@@ -936,9 +862,15 @@
       <xdr:row>31</xdr:row>
       <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -950,25 +882,32 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:srgbClr val="ffff99"/>
+          <a:srgbClr val="FFFF99"/>
         </a:solidFill>
         <a:ln w="9360">
           <a:solidFill>
-            <a:srgbClr val="ffffff"/>
+            <a:srgbClr val="FFFFFF"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000">
+        <a:bodyPr lIns="90000" tIns="45000" rIns="90000" bIns="45000">
           <a:noAutofit/>
         </a:bodyPr>
+        <a:lstStyle/>
         <a:p>
           <a:pPr>
             <a:lnSpc>
@@ -976,7 +915,7 @@
             </a:lnSpc>
           </a:pPr>
           <a:r>
-            <a:rPr b="0" lang="zh-TW" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr lang="zh-TW" sz="1100" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -985,7 +924,7 @@
             <a:t>規格 </a:t>
           </a:r>
           <a:r>
-            <a:rPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+            <a:rPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -993,7 +932,7 @@
             </a:rPr>
             <a:t>: &gt;28.33</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1100" spc="-1" strike="noStrike">
+          <a:endParaRPr lang="en-US" sz="1100" b="0" strike="noStrike" spc="-1">
             <a:latin typeface="Times New Roman"/>
           </a:endParaRPr>
         </a:p>
@@ -1004,33 +943,325 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:U43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="95.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="9"/>
+    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.26953125" style="1" customWidth="1"/>
+    <col min="6" max="7" width="19.453125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.81640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.7265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="95.26953125" style="2" customWidth="1"/>
+    <col min="12" max="1024" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="36.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:21" ht="34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1064,8 +1295,11 @@
       <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="13" customFormat="1">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1088,7 +1322,7 @@
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:21" s="13" customFormat="1">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1111,7 +1345,7 @@
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
     </row>
-    <row r="4" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:21" s="13" customFormat="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1134,7 +1368,7 @@
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
     </row>
-    <row r="5" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:21" s="13" customFormat="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1157,7 +1391,7 @@
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
     </row>
-    <row r="6" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:21" s="14" customFormat="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1180,7 +1414,7 @@
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
     </row>
-    <row r="7" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:21" s="14" customFormat="1">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1203,7 +1437,7 @@
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
     </row>
-    <row r="8" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:21" s="14" customFormat="1">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1226,7 +1460,7 @@
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
     </row>
-    <row r="9" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:21" s="14" customFormat="1">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1249,7 +1483,7 @@
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
     </row>
-    <row r="10" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:21" s="13" customFormat="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="15"/>
@@ -1272,7 +1506,7 @@
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
     </row>
-    <row r="11" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:21" s="13" customFormat="1">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="15"/>
@@ -1295,7 +1529,7 @@
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
     </row>
-    <row r="12" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:21" s="13" customFormat="1">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="15"/>
@@ -1318,7 +1552,7 @@
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
     </row>
-    <row r="13" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:21" s="13" customFormat="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1341,7 +1575,7 @@
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
     </row>
-    <row r="14" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:21" s="13" customFormat="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1364,7 +1598,7 @@
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
     </row>
-    <row r="15" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:21" s="13" customFormat="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1387,7 +1621,7 @@
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
     </row>
-    <row r="16" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:21" s="14" customFormat="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="16"/>
@@ -1410,7 +1644,7 @@
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
     </row>
-    <row r="17" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:21" s="14" customFormat="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="16"/>
@@ -1433,7 +1667,7 @@
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
     </row>
-    <row r="18" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:21" s="14" customFormat="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="16"/>
@@ -1456,7 +1690,7 @@
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
     </row>
-    <row r="19" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:21" s="14" customFormat="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="16"/>
@@ -1479,7 +1713,7 @@
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
     </row>
-    <row r="20" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:21" s="14" customFormat="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="16"/>
@@ -1502,7 +1736,7 @@
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
     </row>
-    <row r="21" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:21" s="14" customFormat="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="16"/>
@@ -1525,7 +1759,7 @@
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
     </row>
-    <row r="22" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:21" s="14" customFormat="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="16"/>
@@ -1548,7 +1782,7 @@
       <c r="T22" s="12"/>
       <c r="U22" s="12"/>
     </row>
-    <row r="23" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:21" s="14" customFormat="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="16"/>
@@ -1571,7 +1805,7 @@
       <c r="T23" s="12"/>
       <c r="U23" s="12"/>
     </row>
-    <row r="24" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:21" s="13" customFormat="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="16"/>
@@ -1594,7 +1828,7 @@
       <c r="T24" s="12"/>
       <c r="U24" s="12"/>
     </row>
-    <row r="25" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:21" s="13" customFormat="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="16"/>
@@ -1617,7 +1851,7 @@
       <c r="T25" s="12"/>
       <c r="U25" s="12"/>
     </row>
-    <row r="26" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:21" s="13" customFormat="1">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="16"/>
@@ -1640,7 +1874,7 @@
       <c r="T26" s="12"/>
       <c r="U26" s="12"/>
     </row>
-    <row r="27" s="13" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:21" s="13" customFormat="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="16"/>
@@ -1663,7 +1897,7 @@
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:21">
       <c r="A28" s="18"/>
       <c r="B28" s="7"/>
       <c r="C28" s="18"/>
@@ -1686,7 +1920,7 @@
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:21">
       <c r="A29" s="18"/>
       <c r="B29" s="7"/>
       <c r="C29" s="18"/>
@@ -1709,7 +1943,7 @@
       <c r="T29" s="12"/>
       <c r="U29" s="12"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:21">
       <c r="A30" s="18"/>
       <c r="B30" s="7"/>
       <c r="C30" s="18"/>
@@ -1732,7 +1966,7 @@
       <c r="T30" s="12"/>
       <c r="U30" s="12"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:21">
       <c r="A31" s="18"/>
       <c r="B31" s="7"/>
       <c r="C31" s="18"/>
@@ -1755,7 +1989,7 @@
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:21">
       <c r="A32" s="18"/>
       <c r="B32" s="7"/>
       <c r="C32" s="18"/>
@@ -1778,7 +2012,7 @@
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:21">
       <c r="A33" s="18"/>
       <c r="B33" s="7"/>
       <c r="C33" s="18"/>
@@ -1801,7 +2035,7 @@
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:21">
       <c r="A34" s="18"/>
       <c r="B34" s="7"/>
       <c r="C34" s="18"/>
@@ -1824,7 +2058,7 @@
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:21">
       <c r="A35" s="18"/>
       <c r="B35" s="7"/>
       <c r="C35" s="18"/>
@@ -1847,7 +2081,7 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:21">
       <c r="A36" s="18"/>
       <c r="B36" s="7"/>
       <c r="C36" s="18"/>
@@ -1870,7 +2104,7 @@
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:21">
       <c r="A37" s="18"/>
       <c r="B37" s="7"/>
       <c r="C37" s="18"/>
@@ -1893,7 +2127,7 @@
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:21">
       <c r="A38" s="18"/>
       <c r="B38" s="7"/>
       <c r="C38" s="18"/>
@@ -1916,7 +2150,7 @@
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:21">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1939,7 +2173,7 @@
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:21">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -1962,7 +2196,7 @@
       <c r="T40" s="12"/>
       <c r="U40" s="12"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:21">
       <c r="A41" s="12"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
@@ -1985,7 +2219,7 @@
       <c r="T41" s="12"/>
       <c r="U41" s="12"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:21">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
@@ -2008,7 +2242,7 @@
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:21">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
@@ -2032,45 +2266,38 @@
       <c r="U43" s="12"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AMJ34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="12.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="21.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="22" width="79.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="20" width="9"/>
+    <col min="1" max="1" width="9" style="20"/>
+    <col min="2" max="2" width="12.90625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9" style="20"/>
+    <col min="4" max="4" width="14" style="20" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="21.36328125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="79.453125" style="22" customWidth="1"/>
+    <col min="12" max="1024" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="54.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" s="29" customFormat="1" ht="51">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2104,8 +2331,11 @@
       <c r="K1" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="29" customFormat="1">
       <c r="A2" s="30"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -2118,7 +2348,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" s="29" customFormat="1">
       <c r="A3" s="30"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -2131,7 +2361,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" s="29" customFormat="1">
       <c r="A4" s="30"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -2144,7 +2374,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12">
       <c r="A5" s="30"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2157,7 +2387,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12">
       <c r="A6" s="30"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -2170,7 +2400,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12">
       <c r="A7" s="30"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -2183,7 +2413,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12">
       <c r="A8" s="30"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -2196,7 +2426,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12">
       <c r="A9" s="30"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -2209,7 +2439,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12">
       <c r="A10" s="30"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2222,7 +2452,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12">
       <c r="A11" s="30"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2235,7 +2465,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12">
       <c r="A12" s="30"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2248,7 +2478,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12">
       <c r="A13" s="30"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2261,7 +2491,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12">
       <c r="A14" s="30"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -2274,7 +2504,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12">
       <c r="A15" s="30"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -2287,7 +2517,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12">
       <c r="A16" s="30"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -2300,7 +2530,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11">
       <c r="A17" s="30"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -2313,7 +2543,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11">
       <c r="A18" s="30"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2326,7 +2556,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11">
       <c r="A19" s="30"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2339,7 +2569,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11">
       <c r="A20" s="30"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -2352,7 +2582,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11">
       <c r="A21" s="30"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -2365,7 +2595,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11">
       <c r="A22" s="30"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2378,7 +2608,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11">
       <c r="A23" s="30"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -2391,7 +2621,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11">
       <c r="A24" s="30"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2404,7 +2634,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11">
       <c r="A25" s="30"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2417,7 +2647,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11">
       <c r="A26" s="30"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2430,7 +2660,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11">
       <c r="A27" s="30"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2443,7 +2673,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11">
       <c r="A28" s="30"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2456,7 +2686,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="11"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11">
       <c r="A29" s="30"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2469,7 +2699,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:11">
       <c r="A30" s="30"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2482,7 +2712,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="11"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:11">
       <c r="A31" s="30"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2495,7 +2725,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="11"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:11">
       <c r="A32" s="30"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2508,7 +2738,7 @@
       <c r="J32" s="8"/>
       <c r="K32" s="33"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:11">
       <c r="A33" s="30"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2521,7 +2751,7 @@
       <c r="J33" s="8"/>
       <c r="K33" s="33"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:11">
       <c r="A34" s="30"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2534,125 +2764,38 @@
       <c r="J34" s="8"/>
       <c r="K34" s="33"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="12.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="22.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="21.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="19.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="22" width="79.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="20" width="9"/>
+    <col min="1" max="1" width="9" style="20"/>
+    <col min="2" max="2" width="12.90625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9" style="20"/>
+    <col min="4" max="4" width="14" style="20" customWidth="1"/>
+    <col min="5" max="5" width="16.6328125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="21.36328125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="79.453125" style="22" customWidth="1"/>
+    <col min="12" max="1024" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" s="29" customFormat="1" ht="51">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -2686,8 +2829,11 @@
       <c r="K1" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="29" customFormat="1">
       <c r="A2" s="30"/>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -2700,7 +2846,7 @@
       <c r="J2" s="37"/>
       <c r="K2" s="39"/>
     </row>
-    <row r="3" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" s="29" customFormat="1">
       <c r="A3" s="30"/>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
@@ -2713,7 +2859,7 @@
       <c r="J3" s="37"/>
       <c r="K3" s="39"/>
     </row>
-    <row r="4" s="29" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" s="29" customFormat="1">
       <c r="A4" s="30"/>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -2726,7 +2872,7 @@
       <c r="J4" s="37"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12">
       <c r="A5" s="30"/>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
@@ -2739,7 +2885,7 @@
       <c r="J5" s="37"/>
       <c r="K5" s="39"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12">
       <c r="A6" s="30"/>
       <c r="B6" s="35"/>
       <c r="C6" s="35"/>
@@ -2752,7 +2898,7 @@
       <c r="J6" s="37"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12">
       <c r="A7" s="30"/>
       <c r="B7" s="35"/>
       <c r="C7" s="35"/>
@@ -2765,7 +2911,7 @@
       <c r="J7" s="37"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12">
       <c r="A8" s="30"/>
       <c r="B8" s="35"/>
       <c r="C8" s="35"/>
@@ -2778,7 +2924,7 @@
       <c r="J8" s="37"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12">
       <c r="A9" s="30"/>
       <c r="B9" s="35"/>
       <c r="C9" s="35"/>
@@ -2791,7 +2937,7 @@
       <c r="J9" s="37"/>
       <c r="K9" s="39"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12">
       <c r="A10" s="30"/>
       <c r="B10" s="35"/>
       <c r="C10" s="35"/>
@@ -2804,7 +2950,7 @@
       <c r="J10" s="37"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12">
       <c r="A11" s="30"/>
       <c r="B11" s="35"/>
       <c r="C11" s="35"/>
@@ -2817,7 +2963,7 @@
       <c r="J11" s="37"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12">
       <c r="A12" s="30"/>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>
@@ -2830,7 +2976,7 @@
       <c r="J12" s="37"/>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12">
       <c r="A13" s="30"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -2843,7 +2989,7 @@
       <c r="J13" s="37"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12">
       <c r="A14" s="30"/>
       <c r="B14" s="35"/>
       <c r="C14" s="35"/>
@@ -2856,7 +3002,7 @@
       <c r="J14" s="37"/>
       <c r="K14" s="39"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12">
       <c r="A15" s="30"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
@@ -2869,7 +3015,7 @@
       <c r="J15" s="37"/>
       <c r="K15" s="39"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12">
       <c r="A16" s="30"/>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
@@ -2882,7 +3028,7 @@
       <c r="J16" s="37"/>
       <c r="K16" s="39"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11">
       <c r="A17" s="30"/>
       <c r="B17" s="35"/>
       <c r="C17" s="35"/>
@@ -2895,7 +3041,7 @@
       <c r="J17" s="37"/>
       <c r="K17" s="39"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11">
       <c r="A18" s="30"/>
       <c r="B18" s="35"/>
       <c r="C18" s="35"/>
@@ -2908,7 +3054,7 @@
       <c r="J18" s="37"/>
       <c r="K18" s="39"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11">
       <c r="A19" s="30"/>
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
@@ -2921,7 +3067,7 @@
       <c r="J19" s="37"/>
       <c r="K19" s="39"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11">
       <c r="A20" s="30"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -2934,7 +3080,7 @@
       <c r="J20" s="37"/>
       <c r="K20" s="39"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11">
       <c r="A21" s="30"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
@@ -2947,7 +3093,7 @@
       <c r="J21" s="37"/>
       <c r="K21" s="39"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11">
       <c r="A22" s="30"/>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
@@ -2960,7 +3106,7 @@
       <c r="J22" s="37"/>
       <c r="K22" s="39"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11">
       <c r="A23" s="30"/>
       <c r="B23" s="35"/>
       <c r="C23" s="35"/>
@@ -2973,7 +3119,7 @@
       <c r="J23" s="37"/>
       <c r="K23" s="39"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11">
       <c r="A24" s="30"/>
       <c r="B24" s="35"/>
       <c r="C24" s="35"/>
@@ -2986,7 +3132,7 @@
       <c r="J24" s="37"/>
       <c r="K24" s="39"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11">
       <c r="A25" s="30"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>
@@ -2999,7 +3145,7 @@
       <c r="J25" s="37"/>
       <c r="K25" s="39"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11">
       <c r="A26" s="30"/>
       <c r="B26" s="35"/>
       <c r="C26" s="35"/>
@@ -3012,7 +3158,7 @@
       <c r="J26" s="37"/>
       <c r="K26" s="39"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11">
       <c r="A27" s="30"/>
       <c r="B27" s="35"/>
       <c r="C27" s="35"/>
@@ -3025,7 +3171,7 @@
       <c r="J27" s="37"/>
       <c r="K27" s="39"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11">
       <c r="A28" s="30"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
@@ -3038,7 +3184,7 @@
       <c r="J28" s="37"/>
       <c r="K28" s="39"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11">
       <c r="A29" s="30"/>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
@@ -3051,7 +3197,7 @@
       <c r="J29" s="37"/>
       <c r="K29" s="39"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:11">
       <c r="A30" s="30"/>
       <c r="B30" s="35"/>
       <c r="C30" s="35"/>
@@ -3064,7 +3210,7 @@
       <c r="J30" s="37"/>
       <c r="K30" s="39"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:11">
       <c r="A31" s="30"/>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
@@ -3077,7 +3223,7 @@
       <c r="J31" s="37"/>
       <c r="K31" s="39"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:11">
       <c r="A32" s="30"/>
       <c r="B32" s="35"/>
       <c r="C32" s="35"/>
@@ -3090,7 +3236,7 @@
       <c r="J32" s="35"/>
       <c r="K32" s="42"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:11">
       <c r="A33" s="30"/>
       <c r="B33" s="35"/>
       <c r="C33" s="35"/>
@@ -3103,7 +3249,7 @@
       <c r="J33" s="35"/>
       <c r="K33" s="42"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:11">
       <c r="A34" s="30"/>
       <c r="B34" s="35"/>
       <c r="C34" s="35"/>
@@ -3116,7 +3262,7 @@
       <c r="J34" s="35"/>
       <c r="K34" s="42"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:11">
       <c r="A35" s="30"/>
       <c r="B35" s="35"/>
       <c r="C35" s="35"/>
@@ -3129,7 +3275,7 @@
       <c r="J35" s="35"/>
       <c r="K35" s="39"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:11">
       <c r="A36" s="30"/>
       <c r="B36" s="37"/>
       <c r="C36" s="35"/>
@@ -3142,7 +3288,7 @@
       <c r="J36" s="35"/>
       <c r="K36" s="39"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:11">
       <c r="A37" s="30"/>
       <c r="B37" s="37"/>
       <c r="C37" s="35"/>
@@ -3155,7 +3301,7 @@
       <c r="J37" s="35"/>
       <c r="K37" s="39"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:11">
       <c r="A38" s="30"/>
       <c r="B38" s="37"/>
       <c r="C38" s="35"/>
@@ -3168,7 +3314,7 @@
       <c r="J38" s="35"/>
       <c r="K38" s="39"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:11">
       <c r="A39" s="30"/>
       <c r="B39" s="37"/>
       <c r="C39" s="35"/>
@@ -3181,7 +3327,7 @@
       <c r="J39" s="35"/>
       <c r="K39" s="39"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:11">
       <c r="A40" s="30"/>
       <c r="B40" s="37"/>
       <c r="C40" s="35"/>
@@ -3194,7 +3340,7 @@
       <c r="J40" s="35"/>
       <c r="K40" s="39"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:11">
       <c r="A41" s="30"/>
       <c r="B41" s="37"/>
       <c r="C41" s="35"/>
@@ -3207,7 +3353,7 @@
       <c r="J41" s="35"/>
       <c r="K41" s="39"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:11">
       <c r="A42" s="30"/>
       <c r="B42" s="37"/>
       <c r="C42" s="35"/>
@@ -3220,7 +3366,7 @@
       <c r="J42" s="35"/>
       <c r="K42" s="39"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:11">
       <c r="A43" s="30"/>
       <c r="B43" s="37"/>
       <c r="C43" s="35"/>
@@ -3233,94 +3379,36 @@
       <c r="J43" s="35"/>
       <c r="K43" s="39"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMJ8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="34.13"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="9"/>
+    <col min="1" max="1" width="14.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.08984375" style="2" customWidth="1"/>
+    <col min="10" max="1024" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="34">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3348,8 +3436,11 @@
       <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="16"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -3360,7 +3451,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10">
       <c r="A3" s="16"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -3371,7 +3462,7 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10">
       <c r="A4" s="16"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -3382,7 +3473,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10">
       <c r="A5" s="16"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -3393,7 +3484,7 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10">
       <c r="A6" s="16"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -3404,7 +3495,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10">
       <c r="A7" s="16"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -3415,7 +3506,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10">
       <c r="A8" s="16"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -3427,40 +3518,33 @@
       <c r="I8" s="18"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="43" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="43" width="8.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="43" width="7.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="43" width="9.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="5" style="43" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="43" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="43" width="77.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="43" width="9"/>
+    <col min="1" max="1" width="12" style="43" customWidth="1"/>
+    <col min="2" max="2" width="8.08984375" style="43" customWidth="1"/>
+    <col min="3" max="3" width="7.6328125" style="43" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" style="43" customWidth="1"/>
+    <col min="5" max="10" width="12" style="43" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" style="43" customWidth="1"/>
+    <col min="12" max="12" width="77.90625" style="43" customWidth="1"/>
+    <col min="13" max="1024" width="9" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13">
       <c r="A1" s="43" t="s">
         <v>21</v>
       </c>
@@ -3497,10 +3581,11 @@
       <c r="L1" s="43" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -3514,7 +3599,7 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13">
       <c r="A5" s="18"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -3528,7 +3613,7 @@
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -3542,7 +3627,7 @@
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -3556,7 +3641,7 @@
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -3570,60 +3655,44 @@
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:13">
       <c r="E11" s="45"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:13">
       <c r="E14" s="45"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="24.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="46" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="46" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="46" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="46" width="28.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="46" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="46" width="32.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="46" width="27.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="46" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="46" width="24.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="46" width="9"/>
+    <col min="1" max="1" width="24.453125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" style="46" customWidth="1"/>
+    <col min="3" max="3" width="10" style="46" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="46" customWidth="1"/>
+    <col min="6" max="6" width="28.36328125" style="46" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" style="46" customWidth="1"/>
+    <col min="8" max="8" width="32.36328125" style="46" customWidth="1"/>
+    <col min="9" max="9" width="27.7265625" style="46" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" style="46" customWidth="1"/>
+    <col min="11" max="11" width="24.453125" style="46" customWidth="1"/>
+    <col min="12" max="1024" width="9" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" ht="34">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3657,8 +3726,11 @@
       <c r="K1" s="51" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21.5">
       <c r="A2" s="52"/>
       <c r="B2" s="53"/>
       <c r="C2" s="54"/>
@@ -3671,7 +3743,7 @@
       <c r="J2" s="54"/>
       <c r="K2" s="55"/>
     </row>
-    <row r="3" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12" ht="21.5">
       <c r="A3" s="52"/>
       <c r="B3" s="53"/>
       <c r="C3" s="54"/>
@@ -3684,7 +3756,7 @@
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
     </row>
-    <row r="4" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12" ht="21.5">
       <c r="A4" s="52"/>
       <c r="B4" s="53"/>
       <c r="C4" s="54"/>
@@ -3697,7 +3769,7 @@
       <c r="J4" s="54"/>
       <c r="K4" s="54"/>
     </row>
-    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12" ht="21.5">
       <c r="A5" s="52"/>
       <c r="B5" s="53"/>
       <c r="C5" s="54"/>
@@ -3710,43 +3782,35 @@
       <c r="J5" s="54"/>
       <c r="K5" s="54"/>
     </row>
-    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="24.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="46" width="21.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="46" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="46" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="46" width="13.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="46" width="27.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="46" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="46" width="45.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="46" width="9"/>
+    <col min="1" max="1" width="24.453125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" style="46" customWidth="1"/>
+    <col min="3" max="3" width="10" style="46" customWidth="1"/>
+    <col min="4" max="4" width="11.08984375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" style="46" customWidth="1"/>
+    <col min="6" max="7" width="27.7265625" style="46" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="46" customWidth="1"/>
+    <col min="9" max="9" width="45.26953125" style="46" customWidth="1"/>
+    <col min="10" max="1024" width="9" style="46"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="34">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
@@ -3774,8 +3838,11 @@
       <c r="I1" s="51" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="56"/>
       <c r="B2" s="57"/>
       <c r="C2" s="56"/>
@@ -3786,7 +3853,7 @@
       <c r="H2" s="56"/>
       <c r="I2" s="58"/>
     </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:10">
       <c r="A3" s="56"/>
       <c r="B3" s="59"/>
       <c r="C3" s="56"/>
@@ -3797,7 +3864,7 @@
       <c r="H3" s="56"/>
       <c r="I3" s="58"/>
     </row>
-    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10">
       <c r="A4" s="56"/>
       <c r="B4" s="59"/>
       <c r="C4" s="56"/>
@@ -3808,7 +3875,7 @@
       <c r="H4" s="56"/>
       <c r="I4" s="58"/>
     </row>
-    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10">
       <c r="A5" s="56"/>
       <c r="B5" s="59"/>
       <c r="C5" s="56"/>
@@ -3819,7 +3886,7 @@
       <c r="H5" s="56"/>
       <c r="I5" s="58"/>
     </row>
-    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10">
       <c r="A6" s="56"/>
       <c r="B6" s="56"/>
       <c r="C6" s="56"/>
@@ -3830,7 +3897,7 @@
       <c r="H6" s="56"/>
       <c r="I6" s="56"/>
     </row>
-    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10">
       <c r="A7" s="56"/>
       <c r="B7" s="56"/>
       <c r="C7" s="56"/>
@@ -3841,7 +3908,7 @@
       <c r="H7" s="56"/>
       <c r="I7" s="56"/>
     </row>
-    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10">
       <c r="A8" s="56"/>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -3852,7 +3919,7 @@
       <c r="H8" s="56"/>
       <c r="I8" s="56"/>
     </row>
-    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10">
       <c r="A9" s="56"/>
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
@@ -3863,7 +3930,7 @@
       <c r="H9" s="56"/>
       <c r="I9" s="56"/>
     </row>
-    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10">
       <c r="A10" s="56"/>
       <c r="B10" s="56"/>
       <c r="C10" s="56"/>
@@ -3874,7 +3941,7 @@
       <c r="H10" s="56"/>
       <c r="I10" s="56"/>
     </row>
-    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10">
       <c r="A11" s="56"/>
       <c r="B11" s="56"/>
       <c r="C11" s="56"/>
@@ -3885,7 +3952,7 @@
       <c r="H11" s="56"/>
       <c r="I11" s="56"/>
     </row>
-    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10">
       <c r="A12" s="56"/>
       <c r="B12" s="56"/>
       <c r="C12" s="56"/>
@@ -3897,43 +3964,36 @@
       <c r="I12" s="56"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.015625" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="12.88"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="20" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="10.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="26.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="20" width="27.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="16.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="22" width="79.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="20" width="9"/>
+    <col min="1" max="1" width="14.36328125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" style="20" customWidth="1"/>
+    <col min="3" max="4" width="9" style="20"/>
+    <col min="5" max="5" width="10.36328125" style="20" customWidth="1"/>
+    <col min="6" max="6" width="26.36328125" style="20" customWidth="1"/>
+    <col min="7" max="7" width="27.26953125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="11.90625" style="20" customWidth="1"/>
+    <col min="11" max="11" width="79.453125" style="22" customWidth="1"/>
+    <col min="12" max="1024" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="true" ht="33" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:12" s="29" customFormat="1" ht="46.5">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
@@ -3967,8 +4027,11 @@
       <c r="K1" s="28" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="23"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3981,7 +4044,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:12">
       <c r="A3" s="23"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -3994,7 +4057,7 @@
       <c r="J3" s="7"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:12">
       <c r="A4" s="23"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4007,7 +4070,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:12">
       <c r="A5" s="23"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4020,7 +4083,7 @@
       <c r="J5" s="63"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:12">
       <c r="A6" s="23"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -4033,7 +4096,7 @@
       <c r="J6" s="63"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:12">
       <c r="A7" s="23"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -4046,7 +4109,7 @@
       <c r="J7" s="63"/>
       <c r="K7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:12">
       <c r="A8" s="23"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -4059,7 +4122,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:12">
       <c r="A9" s="23"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -4072,7 +4135,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:12">
       <c r="A10" s="23"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -4085,7 +4148,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:12">
       <c r="A11" s="23"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
@@ -4098,7 +4161,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:12">
       <c r="A12" s="23"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -4111,7 +4174,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:12">
       <c r="A13" s="23"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -4124,7 +4187,7 @@
       <c r="J13" s="7"/>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:12">
       <c r="A14" s="23"/>
       <c r="B14" s="8"/>
       <c r="C14" s="15"/>
@@ -4137,7 +4200,7 @@
       <c r="J14" s="64"/>
       <c r="K14" s="65"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:12">
       <c r="A15" s="23"/>
       <c r="B15" s="8"/>
       <c r="C15" s="15"/>
@@ -4150,7 +4213,7 @@
       <c r="J15" s="64"/>
       <c r="K15" s="65"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:12">
       <c r="A16" s="23"/>
       <c r="B16" s="64"/>
       <c r="C16" s="15"/>
@@ -4163,7 +4226,7 @@
       <c r="J16" s="64"/>
       <c r="K16" s="65"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:11">
       <c r="A17" s="23"/>
       <c r="B17" s="8"/>
       <c r="C17" s="15"/>
@@ -4176,7 +4239,7 @@
       <c r="J17" s="64"/>
       <c r="K17" s="65"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:11">
       <c r="A18" s="23"/>
       <c r="B18" s="8"/>
       <c r="C18" s="15"/>
@@ -4189,7 +4252,7 @@
       <c r="J18" s="64"/>
       <c r="K18" s="65"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:11">
       <c r="A19" s="23"/>
       <c r="B19" s="64"/>
       <c r="C19" s="15"/>
@@ -4202,7 +4265,7 @@
       <c r="J19" s="64"/>
       <c r="K19" s="65"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:11">
       <c r="A20" s="23"/>
       <c r="B20" s="64"/>
       <c r="C20" s="15"/>
@@ -4215,7 +4278,7 @@
       <c r="J20" s="64"/>
       <c r="K20" s="65"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:11">
       <c r="A21" s="23"/>
       <c r="B21" s="64"/>
       <c r="C21" s="15"/>
@@ -4228,7 +4291,7 @@
       <c r="J21" s="64"/>
       <c r="K21" s="65"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:11">
       <c r="A22" s="23"/>
       <c r="B22" s="64"/>
       <c r="C22" s="15"/>
@@ -4241,7 +4304,7 @@
       <c r="J22" s="64"/>
       <c r="K22" s="65"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:11">
       <c r="A23" s="23"/>
       <c r="B23" s="8"/>
       <c r="C23" s="15"/>
@@ -4254,7 +4317,7 @@
       <c r="J23" s="63"/>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:11">
       <c r="A24" s="23"/>
       <c r="B24" s="63"/>
       <c r="C24" s="15"/>
@@ -4267,7 +4330,7 @@
       <c r="J24" s="63"/>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:11">
       <c r="A25" s="23"/>
       <c r="B25" s="8"/>
       <c r="C25" s="15"/>
@@ -4280,7 +4343,7 @@
       <c r="J25" s="63"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:11">
       <c r="A26" s="23"/>
       <c r="B26" s="8"/>
       <c r="C26" s="15"/>
@@ -4293,7 +4356,7 @@
       <c r="J26" s="63"/>
       <c r="K26" s="11"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:11">
       <c r="A27" s="23"/>
       <c r="B27" s="8"/>
       <c r="C27" s="15"/>
@@ -4306,7 +4369,7 @@
       <c r="J27" s="63"/>
       <c r="K27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:11">
       <c r="A28" s="23"/>
       <c r="B28" s="8"/>
       <c r="C28" s="15"/>
@@ -4319,7 +4382,7 @@
       <c r="J28" s="63"/>
       <c r="K28" s="11"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:11">
       <c r="A29" s="23"/>
       <c r="B29" s="63"/>
       <c r="C29" s="15"/>
@@ -4332,7 +4395,7 @@
       <c r="J29" s="63"/>
       <c r="K29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:11">
       <c r="A30" s="23"/>
       <c r="B30" s="66"/>
       <c r="C30" s="67"/>
@@ -4345,7 +4408,7 @@
       <c r="J30" s="68"/>
       <c r="K30" s="69"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:11">
       <c r="A31" s="23"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -4358,7 +4421,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="71"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:11">
       <c r="A32" s="23"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -4371,7 +4434,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="71"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:11">
       <c r="A33" s="23"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
@@ -4384,7 +4447,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="11"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:11">
       <c r="A34" s="23"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -4397,7 +4460,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="11"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:11">
       <c r="A35" s="23"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -4410,7 +4473,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="11"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:11">
       <c r="A36" s="23"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -4424,13 +4487,9 @@
       <c r="K36" s="11"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <phoneticPr fontId="22" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>